<commit_message>
Confirmação para encerrar app
</commit_message>
<xml_diff>
--- a/regs.xlsx
+++ b/regs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="780" windowWidth="21840" windowHeight="13140" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acts 2021" sheetId="1" state="visible" r:id="rId1"/>
@@ -730,10 +730,10 @@
                 <formatCode>General</formatCode>
                 <ptCount val="2"/>
                 <pt idx="0">
-                  <v>243</v>
+                  <v>252</v>
                 </pt>
                 <pt idx="1">
-                  <v>79</v>
+                  <v>86</v>
                 </pt>
               </numCache>
             </numRef>
@@ -963,7 +963,7 @@
                 <formatCode>General</formatCode>
                 <ptCount val="2"/>
                 <pt idx="0">
-                  <v>320</v>
+                  <v>336</v>
                 </pt>
                 <pt idx="1">
                   <v>8</v>
@@ -1166,10 +1166,10 @@
                 <formatCode>General</formatCode>
                 <ptCount val="8"/>
                 <pt idx="0">
-                  <v>243</v>
+                  <v>252</v>
                 </pt>
                 <pt idx="1">
-                  <v>79</v>
+                  <v>86</v>
                 </pt>
                 <pt idx="2">
                   <v>3</v>
@@ -1181,13 +1181,13 @@
                   <v>6</v>
                 </pt>
                 <pt idx="5">
-                  <v>320</v>
+                  <v>336</v>
                 </pt>
                 <pt idx="6">
                   <v>8</v>
                 </pt>
                 <pt idx="7">
-                  <v>328</v>
+                  <v>344</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2130,7 +2130,7 @@
                 <formatCode>General</formatCode>
                 <ptCount val="1"/>
                 <pt idx="0">
-                  <v>328</v>
+                  <v>344</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2481,7 +2481,7 @@
                 <formatCode>General</formatCode>
                 <ptCount val="1"/>
                 <pt idx="0">
-                  <v>79</v>
+                  <v>86</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2832,7 +2832,7 @@
                 <formatCode>General</formatCode>
                 <ptCount val="1"/>
                 <pt idx="0">
-                  <v>243</v>
+                  <v>252</v>
                 </pt>
               </numCache>
             </numRef>
@@ -23224,8 +23224,8 @@
     <col width="21.6640625" customWidth="1" style="1" min="4" max="4"/>
     <col width="15.109375" customWidth="1" style="1" min="5" max="5"/>
     <col width="19.6640625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="9.109375" customWidth="1" style="1" min="7" max="171"/>
-    <col width="9.109375" customWidth="1" style="1" min="172" max="16384"/>
+    <col width="9.109375" customWidth="1" style="1" min="7" max="173"/>
+    <col width="9.109375" customWidth="1" style="1" min="174" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -37758,8 +37758,8 @@
   </sheetPr>
   <dimension ref="A1:P799"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A454" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A496" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B279" sqref="B279"/>
     </sheetView>
   </sheetViews>
@@ -37773,8 +37773,8 @@
     <col width="23.44140625" customWidth="1" style="1" min="6" max="6"/>
     <col width="16.88671875" customWidth="1" style="1" min="7" max="7"/>
     <col hidden="1" width="9.109375" customWidth="1" style="1" min="8" max="9"/>
-    <col width="9.109375" customWidth="1" style="1" min="10" max="184"/>
-    <col width="9.109375" customWidth="1" style="1" min="185" max="16384"/>
+    <col width="9.109375" customWidth="1" style="1" min="10" max="186"/>
+    <col width="9.109375" customWidth="1" style="1" min="187" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -37814,7 +37814,7 @@
         </is>
       </c>
       <c r="P1" s="1" t="n">
-        <v>510</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2">
@@ -58646,13 +58646,37 @@
       </c>
     </row>
     <row r="510">
-      <c r="A510" s="16" t="n"/>
-      <c r="B510" s="2" t="n"/>
-      <c r="C510" s="16" t="n"/>
-      <c r="D510" s="16" t="n"/>
-      <c r="E510" s="16" t="n"/>
-      <c r="F510" s="21" t="n"/>
-      <c r="G510" s="14" t="n"/>
+      <c r="A510" s="16" t="inlineStr">
+        <is>
+          <t>SUBLIME MOINHOS COMERCIO DE COLCHOES LTDA</t>
+        </is>
+      </c>
+      <c r="B510" s="2" t="n">
+        <v>48189900000155</v>
+      </c>
+      <c r="C510" s="16" t="inlineStr">
+        <is>
+          <t>MR061645/2023</t>
+        </is>
+      </c>
+      <c r="D510" s="16" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="E510" s="16" t="inlineStr">
+        <is>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="F510" s="21" t="inlineStr">
+        <is>
+          <t>01/11/2022 - 31/12/2023</t>
+        </is>
+      </c>
+      <c r="G510" s="22" t="n">
+        <v>45236</v>
+      </c>
       <c r="H510" s="1">
         <f>LEFT(B510,8)</f>
         <v/>
@@ -58663,13 +58687,37 @@
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="16" t="n"/>
-      <c r="B511" s="2" t="n"/>
-      <c r="C511" s="16" t="n"/>
-      <c r="D511" s="16" t="n"/>
-      <c r="E511" s="16" t="n"/>
-      <c r="F511" s="21" t="n"/>
-      <c r="G511" s="14" t="n"/>
+      <c r="A511" s="16" t="inlineStr">
+        <is>
+          <t>SUPERMERCADO PALMITOS LTDA</t>
+        </is>
+      </c>
+      <c r="B511" s="2" t="n">
+        <v>964821000148</v>
+      </c>
+      <c r="C511" s="16" t="inlineStr">
+        <is>
+          <t>MR061010/2023</t>
+        </is>
+      </c>
+      <c r="D511" s="16" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="E511" s="16" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="F511" s="21" t="inlineStr">
+        <is>
+          <t>01/11/2022 - 31/12/2023</t>
+        </is>
+      </c>
+      <c r="G511" s="22" t="n">
+        <v>45236</v>
+      </c>
       <c r="H511" s="1">
         <f>LEFT(B511,8)</f>
         <v/>
@@ -58680,13 +58728,37 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="16" t="n"/>
-      <c r="B512" s="2" t="n"/>
-      <c r="C512" s="16" t="n"/>
-      <c r="D512" s="16" t="n"/>
-      <c r="E512" s="16" t="n"/>
-      <c r="F512" s="21" t="n"/>
-      <c r="G512" s="14" t="n"/>
+      <c r="A512" s="16" t="inlineStr">
+        <is>
+          <t>MINIMERCADO ESCADARIA LTDA</t>
+        </is>
+      </c>
+      <c r="B512" s="2" t="n">
+        <v>7759399000138</v>
+      </c>
+      <c r="C512" s="16" t="inlineStr">
+        <is>
+          <t>MR061002/2023</t>
+        </is>
+      </c>
+      <c r="D512" s="16" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="E512" s="16" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="F512" s="21" t="inlineStr">
+        <is>
+          <t>01/11/2022 - 31/12/2023</t>
+        </is>
+      </c>
+      <c r="G512" s="22" t="n">
+        <v>45236</v>
+      </c>
       <c r="H512" s="1">
         <f>LEFT(B512,8)</f>
         <v/>
@@ -58697,13 +58769,37 @@
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="16" t="n"/>
-      <c r="B513" s="2" t="n"/>
-      <c r="C513" s="16" t="n"/>
-      <c r="D513" s="16" t="n"/>
-      <c r="E513" s="16" t="n"/>
-      <c r="F513" s="21" t="n"/>
-      <c r="G513" s="14" t="n"/>
+      <c r="A513" s="16" t="inlineStr">
+        <is>
+          <t>MADA COMERCIO DE VESTUARIO LTDA</t>
+        </is>
+      </c>
+      <c r="B513" s="2" t="n">
+        <v>37947999000190</v>
+      </c>
+      <c r="C513" s="16" t="inlineStr">
+        <is>
+          <t>MR061242/2023</t>
+        </is>
+      </c>
+      <c r="D513" s="16" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="E513" s="16" t="inlineStr">
+        <is>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="F513" s="21" t="inlineStr">
+        <is>
+          <t>01/11/2022 - 31/12/2023</t>
+        </is>
+      </c>
+      <c r="G513" s="22" t="n">
+        <v>45239</v>
+      </c>
       <c r="H513" s="1">
         <f>LEFT(B513,8)</f>
         <v/>
@@ -58714,13 +58810,37 @@
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="16" t="n"/>
-      <c r="B514" s="2" t="n"/>
-      <c r="C514" s="16" t="n"/>
-      <c r="D514" s="16" t="n"/>
-      <c r="E514" s="16" t="n"/>
-      <c r="F514" s="21" t="n"/>
-      <c r="G514" s="14" t="n"/>
+      <c r="A514" s="16" t="inlineStr">
+        <is>
+          <t>MERCADO MINAS GERAIS LTDA</t>
+        </is>
+      </c>
+      <c r="B514" s="2" t="n">
+        <v>5520581000106</v>
+      </c>
+      <c r="C514" s="16" t="inlineStr">
+        <is>
+          <t>MR022285/2023</t>
+        </is>
+      </c>
+      <c r="D514" s="16" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="E514" s="16" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="F514" s="21" t="inlineStr">
+        <is>
+          <t>01/11/2022 - 31/12/2023</t>
+        </is>
+      </c>
+      <c r="G514" s="22" t="n">
+        <v>45239</v>
+      </c>
       <c r="H514" s="1">
         <f>LEFT(B514,8)</f>
         <v/>
@@ -58731,13 +58851,37 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="16" t="n"/>
-      <c r="B515" s="2" t="n"/>
-      <c r="C515" s="16" t="n"/>
-      <c r="D515" s="16" t="n"/>
-      <c r="E515" s="16" t="n"/>
-      <c r="F515" s="21" t="n"/>
-      <c r="G515" s="14" t="n"/>
+      <c r="A515" s="16" t="inlineStr">
+        <is>
+          <t>KILTY CONFECCOES DE ROUPAS FITNESS LTDA</t>
+        </is>
+      </c>
+      <c r="B515" s="2" t="n">
+        <v>26970989000583</v>
+      </c>
+      <c r="C515" s="16" t="inlineStr">
+        <is>
+          <t>MR062542/2023</t>
+        </is>
+      </c>
+      <c r="D515" s="16" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="E515" s="16" t="inlineStr">
+        <is>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="F515" s="21" t="inlineStr">
+        <is>
+          <t>01/11/2022 - 31/12/2023</t>
+        </is>
+      </c>
+      <c r="G515" s="22" t="n">
+        <v>45243</v>
+      </c>
       <c r="H515" s="1">
         <f>LEFT(B515,8)</f>
         <v/>
@@ -64086,6 +64230,12 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C507" r:id="rId506"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C508" r:id="rId507"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C509" r:id="rId508"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C510" r:id="rId509"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C511" r:id="rId510"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C512" r:id="rId511"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C513" r:id="rId512"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C514" r:id="rId513"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C515" r:id="rId514"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" paperSize="9"/>
@@ -64101,8 +64251,8 @@
   </sheetPr>
   <dimension ref="A1:T183"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -64161,10 +64311,10 @@
         </is>
       </c>
       <c r="S1" t="n">
-        <v>62222</v>
+        <v>63994</v>
       </c>
       <c r="T1" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -66869,20 +67019,20 @@
     <row r="63">
       <c r="A63" s="16" t="inlineStr">
         <is>
-          <t>MERCADO MINAS GERAIS LTDA</t>
+          <t>CESRAN RECRUTAMENTO E SELECAO DE PESSOAL LTDA</t>
         </is>
       </c>
       <c r="B63" s="2" t="n">
-        <v>5520581000106</v>
+        <v>49995556000154</v>
       </c>
       <c r="C63" s="16" t="inlineStr">
         <is>
-          <t>MR022285/2023</t>
+          <t>MR022523/2023</t>
         </is>
       </c>
       <c r="D63" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E63" s="5" t="inlineStr">
@@ -66892,12 +67042,10 @@
       </c>
       <c r="F63" s="5" t="inlineStr">
         <is>
-          <t>Mercado</t>
-        </is>
-      </c>
-      <c r="G63" s="22" t="n">
-        <v>45223</v>
-      </c>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="G63" s="22" t="n"/>
       <c r="H63" s="5">
         <f>IFERROR(VLOOKUP(I63,regs!H:I,2,0),"")</f>
         <v/>
@@ -66914,20 +67062,20 @@
     <row r="64">
       <c r="A64" s="16" t="inlineStr">
         <is>
-          <t>CESRAN RECRUTAMENTO E SELECAO DE PESSOAL LTDA</t>
+          <t>ARMAZEM BOMGADO GA LTDA</t>
         </is>
       </c>
       <c r="B64" s="2" t="n">
-        <v>49995556000154</v>
+        <v>38824899000130</v>
       </c>
       <c r="C64" s="16" t="inlineStr">
         <is>
-          <t>MR022523/2023</t>
+          <t>MR022759/2023</t>
         </is>
       </c>
       <c r="D64" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E64" s="5" t="inlineStr">
@@ -66937,10 +67085,12 @@
       </c>
       <c r="F64" s="5" t="inlineStr">
         <is>
-          <t>Lojista</t>
-        </is>
-      </c>
-      <c r="G64" s="22" t="n"/>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="G64" s="22" t="n">
+        <v>45058</v>
+      </c>
       <c r="H64" s="5">
         <f>IFERROR(VLOOKUP(I64,regs!H:I,2,0),"")</f>
         <v/>
@@ -66957,15 +67107,15 @@
     <row r="65">
       <c r="A65" s="16" t="inlineStr">
         <is>
-          <t>ARMAZEM BOMGADO GA LTDA</t>
+          <t>PAULA H OBJETOS DECORATIVOS E PRESENTES LTDA</t>
         </is>
       </c>
       <c r="B65" s="2" t="n">
-        <v>38824899000130</v>
+        <v>2721404000108</v>
       </c>
       <c r="C65" s="16" t="inlineStr">
         <is>
-          <t>MR022759/2023</t>
+          <t>MR022848/2023</t>
         </is>
       </c>
       <c r="D65" s="5" t="inlineStr">
@@ -66980,11 +67130,11 @@
       </c>
       <c r="F65" s="5" t="inlineStr">
         <is>
-          <t>Mercado</t>
+          <t>Lojista</t>
         </is>
       </c>
       <c r="G65" s="22" t="n">
-        <v>45058</v>
+        <v>45057</v>
       </c>
       <c r="H65" s="5">
         <f>IFERROR(VLOOKUP(I65,regs!H:I,2,0),"")</f>
@@ -67002,15 +67152,15 @@
     <row r="66">
       <c r="A66" s="16" t="inlineStr">
         <is>
-          <t>PAULA H OBJETOS DECORATIVOS E PRESENTES LTDA</t>
+          <t>SERGIO PEDRO TONIOLO</t>
         </is>
       </c>
       <c r="B66" s="2" t="n">
-        <v>2721404000108</v>
+        <v>94678224000109</v>
       </c>
       <c r="C66" s="16" t="inlineStr">
         <is>
-          <t>MR022848/2023</t>
+          <t>MR023039/2023</t>
         </is>
       </c>
       <c r="D66" s="5" t="inlineStr">
@@ -67025,7 +67175,7 @@
       </c>
       <c r="F66" s="5" t="inlineStr">
         <is>
-          <t>Lojista</t>
+          <t>Mercado</t>
         </is>
       </c>
       <c r="G66" s="22" t="n">
@@ -67047,20 +67197,20 @@
     <row r="67">
       <c r="A67" s="16" t="inlineStr">
         <is>
-          <t>SERGIO PEDRO TONIOLO</t>
+          <t>K2 COMERCIO E INDUSTRIA LTDA</t>
         </is>
       </c>
       <c r="B67" s="2" t="n">
-        <v>94678224000109</v>
+        <v>1167639000714</v>
       </c>
       <c r="C67" s="16" t="inlineStr">
         <is>
-          <t>MR023039/2023</t>
+          <t>MR026862/2023</t>
         </is>
       </c>
       <c r="D67" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E67" s="5" t="inlineStr">
@@ -67070,12 +67220,10 @@
       </c>
       <c r="F67" s="5" t="inlineStr">
         <is>
-          <t>Mercado</t>
-        </is>
-      </c>
-      <c r="G67" s="22" t="n">
-        <v>45057</v>
-      </c>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="G67" s="22" t="n"/>
       <c r="H67" s="5">
         <f>IFERROR(VLOOKUP(I67,regs!H:I,2,0),"")</f>
         <v/>
@@ -67092,33 +67240,35 @@
     <row r="68">
       <c r="A68" s="16" t="inlineStr">
         <is>
-          <t>K2 COMERCIO E INDUSTRIA LTDA</t>
+          <t>SINDICATO DOS CONCESSIONARIOS E DISTRIBUIDORES DE VEICULOS NO ESTADO DO RIO GRANDE DO SUL - SINCODIV/RS</t>
         </is>
       </c>
       <c r="B68" s="2" t="n">
-        <v>1167639000714</v>
+        <v>4243203000160</v>
       </c>
       <c r="C68" s="16" t="inlineStr">
         <is>
-          <t>MR026862/2023</t>
+          <t>MR029222/2023</t>
         </is>
       </c>
       <c r="D68" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E68" s="5" t="inlineStr">
         <is>
-          <t>Domingos e feriados</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="F68" s="5" t="inlineStr">
         <is>
-          <t>Lojista</t>
-        </is>
-      </c>
-      <c r="G68" s="22" t="n"/>
+          <t>Indeterminado</t>
+        </is>
+      </c>
+      <c r="G68" s="22" t="n">
+        <v>45084</v>
+      </c>
       <c r="H68" s="5">
         <f>IFERROR(VLOOKUP(I68,regs!H:I,2,0),"")</f>
         <v/>
@@ -67135,15 +67285,15 @@
     <row r="69">
       <c r="A69" s="16" t="inlineStr">
         <is>
-          <t>SINDICATO DOS CONCESSIONARIOS E DISTRIBUIDORES DE VEICULOS NO ESTADO DO RIO GRANDE DO SUL - SINCODIV/RS</t>
+          <t>VISSOMZ ABASTE ESPECIAL DE ESSENCIAS ROGE COMERCIO LTDA</t>
         </is>
       </c>
       <c r="B69" s="2" t="n">
-        <v>4243203000160</v>
+        <v>93866739000161</v>
       </c>
       <c r="C69" s="16" t="inlineStr">
         <is>
-          <t>MR029222/2023</t>
+          <t>MR030541/2023</t>
         </is>
       </c>
       <c r="D69" s="5" t="inlineStr">
@@ -67153,16 +67303,16 @@
       </c>
       <c r="E69" s="5" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Domingos e feriados</t>
         </is>
       </c>
       <c r="F69" s="5" t="inlineStr">
         <is>
-          <t>Indeterminado</t>
+          <t>Lojista</t>
         </is>
       </c>
       <c r="G69" s="22" t="n">
-        <v>45084</v>
+        <v>45103</v>
       </c>
       <c r="H69" s="5">
         <f>IFERROR(VLOOKUP(I69,regs!H:I,2,0),"")</f>
@@ -67180,20 +67330,20 @@
     <row r="70">
       <c r="A70" s="16" t="inlineStr">
         <is>
-          <t>VISSOMZ ABASTE ESPECIAL DE ESSENCIAS ROGE COMERCIO LTDA</t>
+          <t>QDBVISS - ABASTECIMENTO ESPECIAL DE PRODUTOS DE BELEZA LTDA</t>
         </is>
       </c>
       <c r="B70" s="2" t="n">
-        <v>93866739000161</v>
+        <v>19187523000206</v>
       </c>
       <c r="C70" s="16" t="inlineStr">
         <is>
-          <t>MR030541/2023</t>
+          <t>MR030896/2023</t>
         </is>
       </c>
       <c r="D70" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E70" s="5" t="inlineStr">
@@ -67206,9 +67356,7 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G70" s="22" t="n">
-        <v>45103</v>
-      </c>
+      <c r="G70" s="22" t="n"/>
       <c r="H70" s="5">
         <f>IFERROR(VLOOKUP(I70,regs!H:I,2,0),"")</f>
         <v/>
@@ -67225,20 +67373,20 @@
     <row r="71">
       <c r="A71" s="16" t="inlineStr">
         <is>
-          <t>QDBVISS - ABASTECIMENTO ESPECIAL DE PRODUTOS DE BELEZA LTDA</t>
+          <t>AGENSUL - COMERCIO DE PERFUMARIA LTDA</t>
         </is>
       </c>
       <c r="B71" s="2" t="n">
-        <v>19187523000206</v>
+        <v>92916907000113</v>
       </c>
       <c r="C71" s="16" t="inlineStr">
         <is>
-          <t>MR030896/2023</t>
+          <t>MR031783/2023</t>
         </is>
       </c>
       <c r="D71" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E71" s="5" t="inlineStr">
@@ -67251,7 +67399,9 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G71" s="22" t="n"/>
+      <c r="G71" s="22" t="n">
+        <v>45097</v>
+      </c>
       <c r="H71" s="5">
         <f>IFERROR(VLOOKUP(I71,regs!H:I,2,0),"")</f>
         <v/>
@@ -67268,15 +67418,15 @@
     <row r="72">
       <c r="A72" s="16" t="inlineStr">
         <is>
-          <t>AGENSUL - COMERCIO DE PERFUMARIA LTDA</t>
+          <t>DOM COMERCIO DE PERFUMARIA E COSMETICOS LTDA</t>
         </is>
       </c>
       <c r="B72" s="2" t="n">
-        <v>92916907000113</v>
+        <v>14335320000298</v>
       </c>
       <c r="C72" s="16" t="inlineStr">
         <is>
-          <t>MR031783/2023</t>
+          <t>MR031797/2023</t>
         </is>
       </c>
       <c r="D72" s="5" t="inlineStr">
@@ -67313,15 +67463,15 @@
     <row r="73">
       <c r="A73" s="16" t="inlineStr">
         <is>
-          <t>DOM COMERCIO DE PERFUMARIA E COSMETICOS LTDA</t>
+          <t>CH COMERCIO DE PERFUMARIA E COSMETICOS LTDA</t>
         </is>
       </c>
       <c r="B73" s="2" t="n">
-        <v>14335320000298</v>
+        <v>14327879000195</v>
       </c>
       <c r="C73" s="16" t="inlineStr">
         <is>
-          <t>MR031797/2023</t>
+          <t>MR031802/2023</t>
         </is>
       </c>
       <c r="D73" s="5" t="inlineStr">
@@ -67358,20 +67508,20 @@
     <row r="74">
       <c r="A74" s="16" t="inlineStr">
         <is>
-          <t>CH COMERCIO DE PERFUMARIA E COSMETICOS LTDA</t>
+          <t>PITUCHINHUS INDUSTRIA E COMERCIO DE CONFECCOES LTDA</t>
         </is>
       </c>
       <c r="B74" s="2" t="n">
-        <v>14327879000195</v>
+        <v>68765825000564</v>
       </c>
       <c r="C74" s="16" t="inlineStr">
         <is>
-          <t>MR031802/2023</t>
+          <t>MR034407/2023</t>
         </is>
       </c>
       <c r="D74" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E74" s="5" t="inlineStr">
@@ -67384,9 +67534,7 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G74" s="22" t="n">
-        <v>45097</v>
-      </c>
+      <c r="G74" s="22" t="n"/>
       <c r="H74" s="5">
         <f>IFERROR(VLOOKUP(I74,regs!H:I,2,0),"")</f>
         <v/>
@@ -67403,15 +67551,15 @@
     <row r="75">
       <c r="A75" s="16" t="inlineStr">
         <is>
-          <t>PITUCHINHUS INDUSTRIA E COMERCIO DE CONFECCOES LTDA</t>
+          <t>DIAS &amp; CIA LTDA</t>
         </is>
       </c>
       <c r="B75" s="2" t="n">
-        <v>68765825000564</v>
+        <v>3238893000104</v>
       </c>
       <c r="C75" s="16" t="inlineStr">
         <is>
-          <t>MR034407/2023</t>
+          <t>MR035469/2023</t>
         </is>
       </c>
       <c r="D75" s="5" t="inlineStr">
@@ -67446,20 +67594,20 @@
     <row r="76">
       <c r="A76" s="16" t="inlineStr">
         <is>
-          <t>DIAS &amp; CIA LTDA</t>
+          <t>BRASILDECOR MOVEIS E DECORACOES LTDA.</t>
         </is>
       </c>
       <c r="B76" s="2" t="n">
-        <v>3238893000104</v>
+        <v>28709695000285</v>
       </c>
       <c r="C76" s="16" t="inlineStr">
         <is>
-          <t>MR035469/2023</t>
+          <t>MR037779/2023</t>
         </is>
       </c>
       <c r="D76" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E76" s="5" t="inlineStr">
@@ -67472,7 +67620,9 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G76" s="22" t="n"/>
+      <c r="G76" s="22" t="n">
+        <v>45210</v>
+      </c>
       <c r="H76" s="5">
         <f>IFERROR(VLOOKUP(I76,regs!H:I,2,0),"")</f>
         <v/>
@@ -67489,15 +67639,15 @@
     <row r="77">
       <c r="A77" s="16" t="inlineStr">
         <is>
-          <t>BRASILDECOR MOVEIS E DECORACOES LTDA.</t>
+          <t>MOMENTUS TABACARIA LTDA</t>
         </is>
       </c>
       <c r="B77" s="2" t="n">
-        <v>28709695000285</v>
+        <v>44731167000106</v>
       </c>
       <c r="C77" s="16" t="inlineStr">
         <is>
-          <t>MR037779/2023</t>
+          <t>MR022177/2023</t>
         </is>
       </c>
       <c r="D77" s="5" t="inlineStr">
@@ -67516,7 +67666,7 @@
         </is>
       </c>
       <c r="G77" s="22" t="n">
-        <v>45210</v>
+        <v>45068</v>
       </c>
       <c r="H77" s="5">
         <f>IFERROR(VLOOKUP(I77,regs!H:I,2,0),"")</f>
@@ -67534,20 +67684,20 @@
     <row r="78">
       <c r="A78" s="16" t="inlineStr">
         <is>
-          <t>MOMENTUS TABACARIA LTDA</t>
+          <t>GABRIELA DA CUNHA BARBOSA LTDA</t>
         </is>
       </c>
       <c r="B78" s="2" t="n">
-        <v>44731167000106</v>
+        <v>10646336000180</v>
       </c>
       <c r="C78" s="16" t="inlineStr">
         <is>
-          <t>MR022177/2023</t>
+          <t>MR038361/2023</t>
         </is>
       </c>
       <c r="D78" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E78" s="5" t="inlineStr">
@@ -67557,12 +67707,10 @@
       </c>
       <c r="F78" s="5" t="inlineStr">
         <is>
-          <t>Lojista</t>
-        </is>
-      </c>
-      <c r="G78" s="22" t="n">
-        <v>45068</v>
-      </c>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="G78" s="22" t="n"/>
       <c r="H78" s="5">
         <f>IFERROR(VLOOKUP(I78,regs!H:I,2,0),"")</f>
         <v/>
@@ -67579,15 +67727,15 @@
     <row r="79">
       <c r="A79" s="16" t="inlineStr">
         <is>
-          <t>GABRIELA DA CUNHA BARBOSA LTDA</t>
+          <t>C.M. ROZALES COMERCIO DE BRINQUEDOS E DOCES LTDA</t>
         </is>
       </c>
       <c r="B79" s="2" t="n">
-        <v>10646336000180</v>
+        <v>37902619000100</v>
       </c>
       <c r="C79" s="16" t="inlineStr">
         <is>
-          <t>MR038361/2023</t>
+          <t>MR038540/2023</t>
         </is>
       </c>
       <c r="D79" s="5" t="inlineStr">
@@ -67602,7 +67750,7 @@
       </c>
       <c r="F79" s="5" t="inlineStr">
         <is>
-          <t>Mercado</t>
+          <t>Lojista</t>
         </is>
       </c>
       <c r="G79" s="22" t="n"/>
@@ -67622,20 +67770,20 @@
     <row r="80">
       <c r="A80" s="16" t="inlineStr">
         <is>
-          <t>C.M. ROZALES COMERCIO DE BRINQUEDOS E DOCES LTDA</t>
+          <t>MRS COMERCIO DE PRODUTOS REGIONAIS LTDA</t>
         </is>
       </c>
       <c r="B80" s="2" t="n">
-        <v>37902619000100</v>
+        <v>8846951000198</v>
       </c>
       <c r="C80" s="16" t="inlineStr">
         <is>
-          <t>MR038540/2023</t>
+          <t>MR040808/2023</t>
         </is>
       </c>
       <c r="D80" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E80" s="5" t="inlineStr">
@@ -67648,7 +67796,9 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G80" s="22" t="n"/>
+      <c r="G80" s="22" t="n">
+        <v>45139</v>
+      </c>
       <c r="H80" s="5">
         <f>IFERROR(VLOOKUP(I80,regs!H:I,2,0),"")</f>
         <v/>
@@ -67665,20 +67815,20 @@
     <row r="81">
       <c r="A81" s="16" t="inlineStr">
         <is>
-          <t>MRS COMERCIO DE PRODUTOS REGIONAIS LTDA</t>
+          <t>CAMPO VISUAL PARTICIPACOES LTDA</t>
         </is>
       </c>
       <c r="B81" s="2" t="n">
-        <v>8846951000198</v>
+        <v>9248776000108</v>
       </c>
       <c r="C81" s="16" t="inlineStr">
         <is>
-          <t>MR040808/2023</t>
+          <t>MR041737/2023</t>
         </is>
       </c>
       <c r="D81" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E81" s="5" t="inlineStr">
@@ -67688,12 +67838,10 @@
       </c>
       <c r="F81" s="22" t="inlineStr">
         <is>
-          <t>Lojista</t>
-        </is>
-      </c>
-      <c r="G81" s="22" t="n">
-        <v>45139</v>
-      </c>
+          <t>Ótica</t>
+        </is>
+      </c>
+      <c r="G81" s="22" t="n"/>
       <c r="H81" s="5">
         <f>IFERROR(VLOOKUP(I81,regs!H:I,2,0),"")</f>
         <v/>
@@ -67710,15 +67858,15 @@
     <row r="82">
       <c r="A82" s="16" t="inlineStr">
         <is>
-          <t>CAMPO VISUAL PARTICIPACOES LTDA</t>
+          <t>SGH BRASIL COMERCIO DE OCULOS LTDA</t>
         </is>
       </c>
       <c r="B82" s="2" t="n">
-        <v>9248776000108</v>
+        <v>13257648000190</v>
       </c>
       <c r="C82" s="16" t="inlineStr">
         <is>
-          <t>MR041737/2023</t>
+          <t>MR041747/2023</t>
         </is>
       </c>
       <c r="D82" s="5" t="inlineStr">
@@ -67753,20 +67901,20 @@
     <row r="83">
       <c r="A83" s="16" t="inlineStr">
         <is>
-          <t>SGH BRASIL COMERCIO DE OCULOS LTDA</t>
+          <t>JCAM COMERCIO VAREJISTA DE CAPAS E ACESSORIOS LTDA</t>
         </is>
       </c>
       <c r="B83" s="2" t="n">
-        <v>13257648000190</v>
+        <v>27248361000370</v>
       </c>
       <c r="C83" s="16" t="inlineStr">
         <is>
-          <t>MR041747/2023</t>
+          <t>MR042358/2023</t>
         </is>
       </c>
       <c r="D83" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E83" s="5" t="inlineStr">
@@ -67776,10 +67924,12 @@
       </c>
       <c r="F83" s="5" t="inlineStr">
         <is>
-          <t>Ótica</t>
-        </is>
-      </c>
-      <c r="G83" s="22" t="n"/>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="G83" s="22" t="n">
+        <v>45145</v>
+      </c>
       <c r="H83" s="5">
         <f>IFERROR(VLOOKUP(I83,regs!H:I,2,0),"")</f>
         <v/>
@@ -67796,15 +67946,15 @@
     <row r="84">
       <c r="A84" s="16" t="inlineStr">
         <is>
-          <t>JCAM COMERCIO VAREJISTA DE CAPAS E ACESSORIOS LTDA</t>
+          <t>ARMAZEM BOMGADO GA LTDA</t>
         </is>
       </c>
       <c r="B84" s="2" t="n">
-        <v>27248361000370</v>
+        <v>38824899000130</v>
       </c>
       <c r="C84" s="16" t="inlineStr">
         <is>
-          <t>MR042358/2023</t>
+          <t>MR044212/2023</t>
         </is>
       </c>
       <c r="D84" s="5" t="inlineStr">
@@ -67819,7 +67969,7 @@
       </c>
       <c r="F84" s="22" t="inlineStr">
         <is>
-          <t>Lojista</t>
+          <t>Mercado</t>
         </is>
       </c>
       <c r="G84" s="22" t="n">
@@ -67841,15 +67991,15 @@
     <row r="85">
       <c r="A85" s="16" t="inlineStr">
         <is>
-          <t>ARMAZEM BOMGADO GA LTDA</t>
+          <t>J. D. JAQUES</t>
         </is>
       </c>
       <c r="B85" s="2" t="n">
-        <v>38824899000130</v>
+        <v>49312585000174</v>
       </c>
       <c r="C85" s="16" t="inlineStr">
         <is>
-          <t>MR044212/2023</t>
+          <t>MR049127/2023</t>
         </is>
       </c>
       <c r="D85" s="5" t="inlineStr">
@@ -67864,11 +68014,11 @@
       </c>
       <c r="F85" s="22" t="inlineStr">
         <is>
-          <t>Mercado</t>
+          <t>Lojista</t>
         </is>
       </c>
       <c r="G85" s="22" t="n">
-        <v>45145</v>
+        <v>45173</v>
       </c>
       <c r="H85" s="5">
         <f>IFERROR(VLOOKUP(I85,regs!H:I,2,0),"")</f>
@@ -67886,20 +68036,20 @@
     <row r="86">
       <c r="A86" s="16" t="inlineStr">
         <is>
-          <t>J. D. JAQUES</t>
+          <t>L &amp; A COMERCIO DE CALCADOS LTDA</t>
         </is>
       </c>
       <c r="B86" s="2" t="n">
-        <v>49312585000174</v>
+        <v>48748393000223</v>
       </c>
       <c r="C86" s="16" t="inlineStr">
         <is>
-          <t>MR049127/2023</t>
+          <t>MR049502/2023</t>
         </is>
       </c>
       <c r="D86" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E86" s="5" t="inlineStr">
@@ -67912,9 +68062,7 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G86" s="22" t="n">
-        <v>45173</v>
-      </c>
+      <c r="G86" s="22" t="n"/>
       <c r="H86" s="5">
         <f>IFERROR(VLOOKUP(I86,regs!H:I,2,0),"")</f>
         <v/>
@@ -67931,15 +68079,15 @@
     <row r="87">
       <c r="A87" s="16" t="inlineStr">
         <is>
-          <t>L &amp; A COMERCIO DE CALCADOS LTDA</t>
+          <t>M &amp; S COMERCIO DE ALIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B87" s="2" t="n">
-        <v>48748393000223</v>
+        <v>44663036000120</v>
       </c>
       <c r="C87" s="16" t="inlineStr">
         <is>
-          <t>MR049502/2023</t>
+          <t>MR049614/2023</t>
         </is>
       </c>
       <c r="D87" s="5" t="inlineStr">
@@ -67954,7 +68102,7 @@
       </c>
       <c r="F87" s="22" t="inlineStr">
         <is>
-          <t>Lojista</t>
+          <t>Mercado</t>
         </is>
       </c>
       <c r="G87" s="22" t="n"/>
@@ -67974,15 +68122,15 @@
     <row r="88">
       <c r="A88" s="16" t="inlineStr">
         <is>
-          <t>M &amp; S COMERCIO DE ALIMENTOS LTDA</t>
+          <t>MRS COMERCIO DE PRODUTOS REGIONAIS LTDA</t>
         </is>
       </c>
       <c r="B88" s="2" t="n">
-        <v>44663036000120</v>
+        <v>8846951000198</v>
       </c>
       <c r="C88" s="16" t="inlineStr">
         <is>
-          <t>MR049614/2023</t>
+          <t>MR050117/2023</t>
         </is>
       </c>
       <c r="D88" s="5" t="inlineStr">
@@ -67997,7 +68145,7 @@
       </c>
       <c r="F88" s="22" t="inlineStr">
         <is>
-          <t>Mercado</t>
+          <t>Lojista</t>
         </is>
       </c>
       <c r="G88" s="22" t="n"/>
@@ -68017,15 +68165,15 @@
     <row r="89">
       <c r="A89" s="16" t="inlineStr">
         <is>
-          <t>MRS COMERCIO DE PRODUTOS REGIONAIS LTDA</t>
+          <t>ELTON CHRISTMANN</t>
         </is>
       </c>
       <c r="B89" s="2" t="n">
-        <v>8846951000198</v>
+        <v>41733795000124</v>
       </c>
       <c r="C89" s="16" t="inlineStr">
         <is>
-          <t>MR050117/2023</t>
+          <t>MR054169/2023</t>
         </is>
       </c>
       <c r="D89" s="5" t="inlineStr">
@@ -68040,7 +68188,7 @@
       </c>
       <c r="F89" s="22" t="inlineStr">
         <is>
-          <t>Lojista</t>
+          <t>Mercado</t>
         </is>
       </c>
       <c r="G89" s="22" t="n"/>
@@ -68060,15 +68208,15 @@
     <row r="90">
       <c r="A90" s="16" t="inlineStr">
         <is>
-          <t>ELTON CHRISTMANN</t>
+          <t>TERRAS DE AVENTURA INDUSTRIA DE ARTIGOS ESPORTIVOS S.A</t>
         </is>
       </c>
       <c r="B90" s="2" t="n">
-        <v>41733795000124</v>
+        <v>35943604007916</v>
       </c>
       <c r="C90" s="16" t="inlineStr">
         <is>
-          <t>MR054169/2023</t>
+          <t>MR054255/2023</t>
         </is>
       </c>
       <c r="D90" s="5" t="inlineStr">
@@ -68083,7 +68231,7 @@
       </c>
       <c r="F90" s="5" t="inlineStr">
         <is>
-          <t>Mercado</t>
+          <t>Lojista</t>
         </is>
       </c>
       <c r="G90" s="22" t="n"/>
@@ -68103,15 +68251,15 @@
     <row r="91">
       <c r="A91" s="16" t="inlineStr">
         <is>
-          <t>TERRAS DE AVENTURA INDUSTRIA DE ARTIGOS ESPORTIVOS S.A</t>
+          <t>VISSOMZ ABASTE ESPECIAL DE ESSENCIAS ROGE COMERCIO LTDA</t>
         </is>
       </c>
       <c r="B91" s="2" t="n">
-        <v>35943604007916</v>
+        <v>93866739000161</v>
       </c>
       <c r="C91" s="16" t="inlineStr">
         <is>
-          <t>MR054255/2023</t>
+          <t>MR054321/2023</t>
         </is>
       </c>
       <c r="D91" s="5" t="inlineStr">
@@ -68146,15 +68294,15 @@
     <row r="92">
       <c r="A92" s="16" t="inlineStr">
         <is>
-          <t>VISSOMZ ABASTE ESPECIAL DE ESSENCIAS ROGE COMERCIO LTDA</t>
+          <t>JADORE BIJUTERIAS E ACESSORIOS LTDA</t>
         </is>
       </c>
       <c r="B92" s="2" t="n">
-        <v>93866739000161</v>
+        <v>16950484000501</v>
       </c>
       <c r="C92" s="16" t="inlineStr">
         <is>
-          <t>MR054321/2023</t>
+          <t>MR054507/2023</t>
         </is>
       </c>
       <c r="D92" s="5" t="inlineStr">
@@ -68189,15 +68337,15 @@
     <row r="93">
       <c r="A93" s="16" t="inlineStr">
         <is>
-          <t>JADORE BIJUTERIAS E ACESSORIOS LTDA</t>
+          <t>R. JAQUES DE ANDRADE</t>
         </is>
       </c>
       <c r="B93" s="2" t="n">
-        <v>16950484000501</v>
+        <v>38824968000105</v>
       </c>
       <c r="C93" s="16" t="inlineStr">
         <is>
-          <t>MR054507/2023</t>
+          <t>MR054671/2023</t>
         </is>
       </c>
       <c r="D93" s="5" t="inlineStr">
@@ -68232,15 +68380,15 @@
     <row r="94">
       <c r="A94" s="16" t="inlineStr">
         <is>
-          <t>R. JAQUES DE ANDRADE</t>
+          <t>THAIS ANGELICA FOLLMANN BENNEMANN LTDA</t>
         </is>
       </c>
       <c r="B94" s="2" t="n">
-        <v>38824968000105</v>
+        <v>51188904000123</v>
       </c>
       <c r="C94" s="16" t="inlineStr">
         <is>
-          <t>MR054671/2023</t>
+          <t>MR055140/2023</t>
         </is>
       </c>
       <c r="D94" s="5" t="inlineStr">
@@ -68275,15 +68423,15 @@
     <row r="95">
       <c r="A95" s="16" t="inlineStr">
         <is>
-          <t>THAIS ANGELICA FOLLMANN BENNEMANN LTDA</t>
+          <t>REAL COMERCIAL LTDA</t>
         </is>
       </c>
       <c r="B95" s="2" t="n">
-        <v>51188904000123</v>
+        <v>2780640000197</v>
       </c>
       <c r="C95" s="16" t="inlineStr">
         <is>
-          <t>MR055140/2023</t>
+          <t>MR055548/2023</t>
         </is>
       </c>
       <c r="D95" s="5" t="inlineStr">
@@ -68298,7 +68446,7 @@
       </c>
       <c r="F95" s="22" t="inlineStr">
         <is>
-          <t>Lojista</t>
+          <t>Mercado</t>
         </is>
       </c>
       <c r="G95" s="22" t="n"/>
@@ -68318,20 +68466,20 @@
     <row r="96">
       <c r="A96" s="16" t="inlineStr">
         <is>
-          <t>REAL COMERCIAL LTDA</t>
+          <t>FL TECH INFORMATICA LTDA</t>
         </is>
       </c>
       <c r="B96" s="2" t="n">
-        <v>2780640000197</v>
+        <v>46964709000108</v>
       </c>
       <c r="C96" s="16" t="inlineStr">
         <is>
-          <t>MR055548/2023</t>
+          <t>MR055557/2023</t>
         </is>
       </c>
       <c r="D96" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E96" s="5" t="inlineStr">
@@ -68341,10 +68489,12 @@
       </c>
       <c r="F96" s="22" t="inlineStr">
         <is>
-          <t>Mercado</t>
-        </is>
-      </c>
-      <c r="G96" s="22" t="n"/>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="G96" s="22" t="n">
+        <v>45239</v>
+      </c>
       <c r="H96" s="5">
         <f>IFERROR(VLOOKUP(I96,regs!H:I,2,0),"")</f>
         <v/>
@@ -68361,20 +68511,20 @@
     <row r="97">
       <c r="A97" s="16" t="inlineStr">
         <is>
-          <t>FL TECH INFORMATICA LTDA</t>
+          <t>NIZZA COMERCIO DE CONFECCOES LTDA</t>
         </is>
       </c>
       <c r="B97" s="2" t="n">
-        <v>46964709000108</v>
+        <v>42160869000143</v>
       </c>
       <c r="C97" s="16" t="inlineStr">
         <is>
-          <t>MR055557/2023</t>
+          <t>MR055577/2023</t>
         </is>
       </c>
       <c r="D97" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E97" s="5" t="inlineStr">
@@ -68387,7 +68537,9 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G97" s="22" t="n"/>
+      <c r="G97" s="22" t="n">
+        <v>45210</v>
+      </c>
       <c r="H97" s="5">
         <f>IFERROR(VLOOKUP(I97,regs!H:I,2,0),"")</f>
         <v/>
@@ -68404,15 +68556,15 @@
     <row r="98">
       <c r="A98" s="16" t="inlineStr">
         <is>
-          <t>NIZZA COMERCIO DE CONFECCOES LTDA</t>
+          <t>BOOMER COMERCIO DE CONFECCOES LTDA</t>
         </is>
       </c>
       <c r="B98" s="2" t="n">
-        <v>42160869000143</v>
+        <v>28613652000200</v>
       </c>
       <c r="C98" s="16" t="inlineStr">
         <is>
-          <t>MR055577/2023</t>
+          <t>MR055583/2023</t>
         </is>
       </c>
       <c r="D98" s="5" t="inlineStr">
@@ -68449,15 +68601,15 @@
     <row r="99">
       <c r="A99" s="16" t="inlineStr">
         <is>
-          <t>BOOMER COMERCIO DE CONFECCOES LTDA</t>
+          <t>LERNER COMERCIO E ASSISTENCIA TECNICA DE CELULARES LTDA</t>
         </is>
       </c>
       <c r="B99" s="2" t="n">
-        <v>28613652000200</v>
+        <v>50767215000100</v>
       </c>
       <c r="C99" s="16" t="inlineStr">
         <is>
-          <t>MR055583/2023</t>
+          <t>MR056814/2023</t>
         </is>
       </c>
       <c r="D99" s="5" t="inlineStr">
@@ -68476,7 +68628,7 @@
         </is>
       </c>
       <c r="G99" s="22" t="n">
-        <v>45210</v>
+        <v>45204</v>
       </c>
       <c r="H99" s="5">
         <f>IFERROR(VLOOKUP(I99,regs!H:I,2,0),"")</f>
@@ -68494,15 +68646,15 @@
     <row r="100">
       <c r="A100" s="16" t="inlineStr">
         <is>
-          <t>LERNER COMERCIO E ASSISTENCIA TECNICA DE CELULARES LTDA</t>
+          <t>MAX CENTER CENTRO DE COMPRAS LTDA</t>
         </is>
       </c>
       <c r="B100" s="2" t="n">
-        <v>50767215000100</v>
+        <v>8769595000407</v>
       </c>
       <c r="C100" s="16" t="inlineStr">
         <is>
-          <t>MR056814/2023</t>
+          <t>MR059494/2023</t>
         </is>
       </c>
       <c r="D100" s="5" t="inlineStr">
@@ -68517,11 +68669,11 @@
       </c>
       <c r="F100" s="5" t="inlineStr">
         <is>
-          <t>Lojista</t>
+          <t>Mercado</t>
         </is>
       </c>
       <c r="G100" s="22" t="n">
-        <v>45204</v>
+        <v>45233</v>
       </c>
       <c r="H100" s="5">
         <f>IFERROR(VLOOKUP(I100,regs!H:I,2,0),"")</f>
@@ -68539,15 +68691,15 @@
     <row r="101">
       <c r="A101" s="16" t="inlineStr">
         <is>
-          <t>MAX CENTER CENTRO DE COMPRAS LTDA</t>
+          <t>SUPERMERCADO FLACH LTDA</t>
         </is>
       </c>
       <c r="B101" s="2" t="n">
-        <v>8769595000407</v>
+        <v>88692314000143</v>
       </c>
       <c r="C101" s="16" t="inlineStr">
         <is>
-          <t>MR059494/2023</t>
+          <t>MR059749/2023</t>
         </is>
       </c>
       <c r="D101" s="5" t="inlineStr">
@@ -68566,7 +68718,7 @@
         </is>
       </c>
       <c r="G101" s="22" t="n">
-        <v>45233</v>
+        <v>45223</v>
       </c>
       <c r="H101" s="5">
         <f>IFERROR(VLOOKUP(I101,regs!H:I,2,0),"")</f>
@@ -68584,15 +68736,15 @@
     <row r="102">
       <c r="A102" s="16" t="inlineStr">
         <is>
-          <t>SUPERMERCADO FLACH LTDA</t>
+          <t>ALBERTI COMERCIO DE ALIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B102" s="2" t="n">
-        <v>88692314000143</v>
+        <v>1254300000160</v>
       </c>
       <c r="C102" s="16" t="inlineStr">
         <is>
-          <t>MR059749/2023</t>
+          <t>MR061063/2023</t>
         </is>
       </c>
       <c r="D102" s="5" t="inlineStr">
@@ -68611,7 +68763,7 @@
         </is>
       </c>
       <c r="G102" s="22" t="n">
-        <v>45223</v>
+        <v>45229</v>
       </c>
       <c r="H102" s="5">
         <f>IFERROR(VLOOKUP(I102,regs!H:I,2,0),"")</f>
@@ -68629,15 +68781,15 @@
     <row r="103">
       <c r="A103" s="16" t="inlineStr">
         <is>
-          <t>MINIMERCADO ESCADARIA LTDA</t>
+          <t>J B VIEIRA COMERCIO DE ALIMENTOS LTDA</t>
         </is>
       </c>
       <c r="B103" s="2" t="n">
-        <v>7759399000138</v>
+        <v>25535075000106</v>
       </c>
       <c r="C103" s="16" t="inlineStr">
         <is>
-          <t>MR061002/2023</t>
+          <t>MR061073/2023</t>
         </is>
       </c>
       <c r="D103" s="5" t="inlineStr">
@@ -68674,15 +68826,15 @@
     <row r="104">
       <c r="A104" s="16" t="inlineStr">
         <is>
-          <t>ALBERTI COMERCIO DE ALIMENTOS LTDA</t>
+          <t>ROZA SERENA COMERCIO DE CALCADOS LTDA</t>
         </is>
       </c>
       <c r="B104" s="2" t="n">
-        <v>1254300000160</v>
+        <v>52172316000164</v>
       </c>
       <c r="C104" s="16" t="inlineStr">
         <is>
-          <t>MR061063/2023</t>
+          <t>MR061404/2023</t>
         </is>
       </c>
       <c r="D104" s="5" t="inlineStr">
@@ -68697,11 +68849,11 @@
       </c>
       <c r="F104" s="22" t="inlineStr">
         <is>
-          <t>Mercado</t>
+          <t>Lojista</t>
         </is>
       </c>
       <c r="G104" s="22" t="n">
-        <v>45229</v>
+        <v>45240</v>
       </c>
       <c r="H104" s="5">
         <f>IFERROR(VLOOKUP(I104,regs!H:I,2,0),"")</f>
@@ -68719,20 +68871,20 @@
     <row r="105">
       <c r="A105" s="16" t="inlineStr">
         <is>
-          <t>J B VIEIRA COMERCIO DE ALIMENTOS LTDA</t>
+          <t>G. TRICOT POA COMERCIO DE ARTIGOS DE VESTUARIO LTDA</t>
         </is>
       </c>
       <c r="B105" s="2" t="n">
-        <v>25535075000106</v>
+        <v>51603161000100</v>
       </c>
       <c r="C105" s="16" t="inlineStr">
         <is>
-          <t>MR061073/2023</t>
+          <t>MR061715/2023</t>
         </is>
       </c>
       <c r="D105" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E105" s="5" t="inlineStr">
@@ -68742,12 +68894,10 @@
       </c>
       <c r="F105" s="22" t="inlineStr">
         <is>
-          <t>Mercado</t>
-        </is>
-      </c>
-      <c r="G105" s="22" t="n">
-        <v>45229</v>
-      </c>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="G105" s="22" t="n"/>
       <c r="H105" s="5">
         <f>IFERROR(VLOOKUP(I105,regs!H:I,2,0),"")</f>
         <v/>
@@ -68764,20 +68914,20 @@
     <row r="106">
       <c r="A106" s="16" t="inlineStr">
         <is>
-          <t>MADA COMERCIO DE VESTUARIO LTDA</t>
+          <t>CALCADOS TOMAZZINI LTDA</t>
         </is>
       </c>
       <c r="B106" s="2" t="n">
-        <v>37947999000190</v>
+        <v>47612500000300</v>
       </c>
       <c r="C106" s="16" t="inlineStr">
         <is>
-          <t>MR061242/2023</t>
+          <t>MR062287/2023</t>
         </is>
       </c>
       <c r="D106" s="5" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NÃO</t>
         </is>
       </c>
       <c r="E106" s="5" t="inlineStr">
@@ -68790,9 +68940,7 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G106" s="22" t="n">
-        <v>45230</v>
-      </c>
+      <c r="G106" s="22" t="n"/>
       <c r="H106" s="5">
         <f>IFERROR(VLOOKUP(I106,regs!H:I,2,0),"")</f>
         <v/>
@@ -68809,20 +68957,20 @@
     <row r="107">
       <c r="A107" s="16" t="inlineStr">
         <is>
-          <t>ROZA SERENA COMERCIO DE CALCADOS LTDA</t>
+          <t>OFF STORE COMERCIO DE MOVEIS LTDA</t>
         </is>
       </c>
       <c r="B107" s="2" t="n">
-        <v>52172316000164</v>
+        <v>7827077000260</v>
       </c>
       <c r="C107" s="16" t="inlineStr">
         <is>
-          <t>MR061404/2023</t>
+          <t>MR062658/2023</t>
         </is>
       </c>
       <c r="D107" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E107" s="5" t="inlineStr">
@@ -68835,7 +68983,9 @@
           <t>Lojista</t>
         </is>
       </c>
-      <c r="G107" s="22" t="inlineStr"/>
+      <c r="G107" s="22" t="n">
+        <v>45239</v>
+      </c>
       <c r="H107" s="5">
         <f>IFERROR(VLOOKUP(I107,regs!H:I,2,0),"")</f>
         <v/>
@@ -68852,20 +69002,20 @@
     <row r="108">
       <c r="A108" s="16" t="inlineStr">
         <is>
-          <t>G. TRICOT POA COMERCIO DE ARTIGOS DE VESTUARIO LTDA</t>
+          <t>W &amp; F COMERCIO DE MOVEIS LTDA</t>
         </is>
       </c>
       <c r="B108" s="2" t="n">
-        <v>51603161000100</v>
+        <v>35624688000165</v>
       </c>
       <c r="C108" s="16" t="inlineStr">
         <is>
-          <t>MR061715/2023</t>
+          <t>MR062666/2023</t>
         </is>
       </c>
       <c r="D108" s="5" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="E108" s="5" t="inlineStr">
@@ -68873,12 +69023,14 @@
           <t>Domingos e feriados</t>
         </is>
       </c>
-      <c r="F108" s="5" t="inlineStr">
-        <is>
-          <t>Lojista</t>
-        </is>
-      </c>
-      <c r="G108" s="22" t="inlineStr"/>
+      <c r="F108" s="22" t="inlineStr">
+        <is>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="G108" s="22" t="n">
+        <v>45239</v>
+      </c>
       <c r="H108" s="5">
         <f>IFERROR(VLOOKUP(I108,regs!H:I,2,0),"")</f>
         <v/>
@@ -68893,12 +69045,34 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="16" t="n"/>
-      <c r="B109" s="2" t="n"/>
-      <c r="C109" s="16" t="n"/>
-      <c r="D109" s="5" t="n"/>
-      <c r="E109" s="5" t="n"/>
-      <c r="F109" s="5" t="n"/>
+      <c r="A109" s="16" t="inlineStr">
+        <is>
+          <t>PAISAGEM LIVRARIA, PAPELARIA E ARTIGOS DE DECORACAO LTDA</t>
+        </is>
+      </c>
+      <c r="B109" s="2" t="n">
+        <v>41778264000310</v>
+      </c>
+      <c r="C109" s="16" t="inlineStr">
+        <is>
+          <t>MR063103/2023</t>
+        </is>
+      </c>
+      <c r="D109" s="5" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="E109" s="5" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="F109" s="22" t="inlineStr">
+        <is>
+          <t>Lojista</t>
+        </is>
+      </c>
       <c r="G109" s="22" t="n"/>
       <c r="H109" s="5">
         <f>IFERROR(VLOOKUP(I109,regs!H:I,2,0),"")</f>
@@ -68914,13 +69088,37 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="16" t="n"/>
-      <c r="B110" s="2" t="n"/>
-      <c r="C110" s="16" t="n"/>
-      <c r="D110" s="5" t="n"/>
-      <c r="E110" s="5" t="n"/>
-      <c r="F110" s="5" t="n"/>
-      <c r="G110" s="22" t="n"/>
+      <c r="A110" s="16" t="inlineStr">
+        <is>
+          <t>IMCOSUL LOJA DE DEPARTAMENTOS LTDA</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>40884352000171</v>
+      </c>
+      <c r="C110" s="16" t="inlineStr">
+        <is>
+          <t>MR063671/2023</t>
+        </is>
+      </c>
+      <c r="D110" s="5" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="E110" s="5" t="inlineStr">
+        <is>
+          <t>Domingos e feriados</t>
+        </is>
+      </c>
+      <c r="F110" s="5" t="inlineStr">
+        <is>
+          <t>Lojista</t>
+        </is>
+      </c>
+      <c r="G110" s="22" t="n">
+        <v>45243</v>
+      </c>
       <c r="H110" s="5">
         <f>IFERROR(VLOOKUP(I110,regs!H:I,2,0),"")</f>
         <v/>
@@ -68935,13 +69133,13 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="16" t="n"/>
-      <c r="B111" s="2" t="n"/>
-      <c r="C111" s="16" t="n"/>
-      <c r="D111" s="5" t="n"/>
-      <c r="E111" s="5" t="n"/>
-      <c r="F111" s="5" t="n"/>
-      <c r="G111" s="22" t="n"/>
+      <c r="A111" s="16" t="inlineStr"/>
+      <c r="B111" s="2" t="inlineStr"/>
+      <c r="C111" s="16" t="inlineStr"/>
+      <c r="D111" s="5" t="inlineStr"/>
+      <c r="E111" s="5" t="inlineStr"/>
+      <c r="F111" s="5" t="inlineStr"/>
+      <c r="G111" s="22" t="inlineStr"/>
       <c r="H111" s="5">
         <f>IFERROR(VLOOKUP(I111,regs!H:I,2,0),"")</f>
         <v/>
@@ -70545,7 +70743,7 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
@@ -70654,7 +70852,7 @@
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>

</xml_diff>